<commit_message>
Update file from SharePoint:
</commit_message>
<xml_diff>
--- a/Mailbox Emails/Mailbox Emails.xlsx
+++ b/Mailbox Emails/Mailbox Emails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pressassociation.sharepoint.com/sites/ServicesTeam/Shared Documents/Mailbox Emails/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2047" documentId="8_{0B395730-64AC-4FF2-BF32-032FEAA45924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8731218D-DE01-4DC4-BB05-9752753DB227}"/>
+  <xr:revisionPtr revIDLastSave="2073" documentId="8_{0B395730-64AC-4FF2-BF32-032FEAA45924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2576F9D-86B2-4D95-BCAB-84F617209E53}"/>
   <bookViews>
-    <workbookView xWindow="4284" yWindow="6384" windowWidth="23052" windowHeight="13140" xr2:uid="{1F2C4778-E4C2-4806-9BD6-AC1A533EA935}"/>
+    <workbookView xWindow="4280" yWindow="3440" windowWidth="23060" windowHeight="13140" xr2:uid="{1F2C4778-E4C2-4806-9BD6-AC1A533EA935}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6112" uniqueCount="2935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6190" uniqueCount="2970">
   <si>
     <t>received_date_time</t>
   </si>
@@ -8841,6 +8841,111 @@
   </si>
   <si>
     <t>2025-07-24T18:01:47+00:00</t>
+  </si>
+  <si>
+    <t>2025-07-24T19:16:15+00:00</t>
+  </si>
+  <si>
+    <t>2025-07-24T19:16:13+00:00</t>
+  </si>
+  <si>
+    <t>2025-07-24T19:16:07+00:00</t>
+  </si>
+  <si>
+    <t>2025-07-24T19:15:59+00:00</t>
+  </si>
+  <si>
+    <t>2025-07-24T19:15:58+00:00</t>
+  </si>
+  <si>
+    <t>2025-07-24T19:15:56+00:00</t>
+  </si>
+  <si>
+    <t>2025-07-24T19:15:47+00:00</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:15:50+00:00</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:01:30+00:00</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:01:15+00:00</t>
+  </si>
+  <si>
+    <t>EXTERNAL:- BBC Asian Network - Wk33 - 2025-08-22 - Friday</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:01:11+00:00</t>
+  </si>
+  <si>
+    <t>EXTERNAL:- BBC Radio 3 - Wk33 - 2025-08-19 - Tuesday</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:01:08+00:00</t>
+  </si>
+  <si>
+    <t>EXTERNAL:- BBC Radio 3 - Wk33 - 2025-08-21 - Thursday</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:01:07+00:00</t>
+  </si>
+  <si>
+    <t>EXTERNAL:- BBC Radio 1Xtra - Wk33 - 2025-08-20 - Wednesday</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:01:03+00:00</t>
+  </si>
+  <si>
+    <t>EXTERNAL:- BBC Asian Network - Wk33 - 2025-08-20 - Wednesday</t>
+  </si>
+  <si>
+    <t>EXTERNAL:- BBC Radio 6 Music - Wk33 - 2025-08-19 - Tuesday</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:01:01+00:00</t>
+  </si>
+  <si>
+    <t>EXTERNAL:- BBC Radio 2 - Wk33 - 2025-08-19 - Tuesday</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:00:59+00:00</t>
+  </si>
+  <si>
+    <t>EXTERNAL:- BBC Asian Network - Wk33 - 2025-08-18 - Monday</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:00:54+00:00</t>
+  </si>
+  <si>
+    <t>EXTERNAL:- BBC Radio 2 - Wk33 - 2025-08-17 - Sunday</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:00:52+00:00</t>
+  </si>
+  <si>
+    <t>EXTERNAL:- BBC Radio 4 FM - Wk32 - 2025-08-13 - Wednesday</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:00:51+00:00</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:00:43+00:00</t>
+  </si>
+  <si>
+    <t>EXTERNAL:- BBC Radio 5 Sports Extra - Wk32 - 2025-08-12 - Tuesday</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:00:38+00:00</t>
+  </si>
+  <si>
+    <t>EXTERNAL:- BBC Radio 1Xtra - Wk32 - 2025-08-10 - Sunday</t>
+  </si>
+  <si>
+    <t>2025-07-24T20:00:36+00:00</t>
+  </si>
+  <si>
+    <t>EXTERNAL:- BBC Radio 1Xtra - Wk31 - 2025-08-05 - Tuesday</t>
   </si>
 </sst>
 </file>
@@ -8896,8 +9001,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{30666ACE-24FE-4456-8444-66338A7177B0}" name="Table1" displayName="Table1" ref="A1:D2037" totalsRowShown="0">
-  <autoFilter ref="A1:D2037" xr:uid="{30666ACE-24FE-4456-8444-66338A7177B0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{30666ACE-24FE-4456-8444-66338A7177B0}" name="Table1" displayName="Table1" ref="A1:D2063" totalsRowShown="0">
+  <autoFilter ref="A1:D2063" xr:uid="{30666ACE-24FE-4456-8444-66338A7177B0}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0C1DF6AA-30FA-4D4F-89E6-B18A63B96047}" name="received_date_time"/>
     <tableColumn id="2" xr3:uid="{361C10ED-A6EC-45C8-B5B5-E722DB38A1CE}" name="subject"/>
@@ -9225,18 +9330,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E4D268B-372D-4A16-AE6F-A065FA20C63D}">
-  <dimension ref="A1:D2037"/>
+  <dimension ref="A1:D2063"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -37754,6 +37859,370 @@
         <v>12</v>
       </c>
       <c r="D2037" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2038" spans="1:4">
+      <c r="A2038" t="s">
+        <v>2935</v>
+      </c>
+      <c r="B2038" t="s">
+        <v>2129</v>
+      </c>
+      <c r="C2038" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2038" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2039" spans="1:4">
+      <c r="A2039" t="s">
+        <v>2935</v>
+      </c>
+      <c r="B2039" t="s">
+        <v>2322</v>
+      </c>
+      <c r="C2039" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2039" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2040" spans="1:4">
+      <c r="A2040" t="s">
+        <v>2936</v>
+      </c>
+      <c r="B2040" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C2040" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2040" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2041" spans="1:4">
+      <c r="A2041" t="s">
+        <v>2937</v>
+      </c>
+      <c r="B2041" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C2041" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2041" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2042" spans="1:4">
+      <c r="A2042" t="s">
+        <v>2938</v>
+      </c>
+      <c r="B2042" t="s">
+        <v>2555</v>
+      </c>
+      <c r="C2042" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2042" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2043" spans="1:4">
+      <c r="A2043" t="s">
+        <v>2939</v>
+      </c>
+      <c r="B2043" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2043" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2043" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2044" spans="1:4">
+      <c r="A2044" t="s">
+        <v>2939</v>
+      </c>
+      <c r="B2044" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2044" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2044" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2045" spans="1:4">
+      <c r="A2045" t="s">
+        <v>2940</v>
+      </c>
+      <c r="B2045" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C2045" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2045" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2046" spans="1:4">
+      <c r="A2046" t="s">
+        <v>2940</v>
+      </c>
+      <c r="B2046" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2046" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2046" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2047" spans="1:4">
+      <c r="A2047" t="s">
+        <v>2941</v>
+      </c>
+      <c r="B2047" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2047" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2047" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2048" spans="1:4">
+      <c r="A2048" t="s">
+        <v>2942</v>
+      </c>
+      <c r="B2048" t="s">
+        <v>649</v>
+      </c>
+      <c r="C2048" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2048" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2049" spans="1:4">
+      <c r="A2049" t="s">
+        <v>2943</v>
+      </c>
+      <c r="B2049" t="s">
+        <v>2097</v>
+      </c>
+      <c r="C2049" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2049" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2050" spans="1:4">
+      <c r="A2050" t="s">
+        <v>2944</v>
+      </c>
+      <c r="B2050" t="s">
+        <v>2945</v>
+      </c>
+      <c r="C2050" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2050" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2051" spans="1:4">
+      <c r="A2051" t="s">
+        <v>2946</v>
+      </c>
+      <c r="B2051" t="s">
+        <v>2947</v>
+      </c>
+      <c r="C2051" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2051" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2052" spans="1:4">
+      <c r="A2052" t="s">
+        <v>2948</v>
+      </c>
+      <c r="B2052" t="s">
+        <v>2949</v>
+      </c>
+      <c r="C2052" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2052" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2053" spans="1:4">
+      <c r="A2053" t="s">
+        <v>2950</v>
+      </c>
+      <c r="B2053" t="s">
+        <v>2951</v>
+      </c>
+      <c r="C2053" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2053" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2054" spans="1:4">
+      <c r="A2054" t="s">
+        <v>2952</v>
+      </c>
+      <c r="B2054" t="s">
+        <v>2953</v>
+      </c>
+      <c r="C2054" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2054" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2055" spans="1:4">
+      <c r="A2055" t="s">
+        <v>2952</v>
+      </c>
+      <c r="B2055" t="s">
+        <v>2954</v>
+      </c>
+      <c r="C2055" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2055" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2056" spans="1:4">
+      <c r="A2056" t="s">
+        <v>2955</v>
+      </c>
+      <c r="B2056" t="s">
+        <v>2956</v>
+      </c>
+      <c r="C2056" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2056" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2057" spans="1:4">
+      <c r="A2057" t="s">
+        <v>2957</v>
+      </c>
+      <c r="B2057" t="s">
+        <v>2958</v>
+      </c>
+      <c r="C2057" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2057" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2058" spans="1:4">
+      <c r="A2058" t="s">
+        <v>2959</v>
+      </c>
+      <c r="B2058" t="s">
+        <v>2960</v>
+      </c>
+      <c r="C2058" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2058" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2059" spans="1:4">
+      <c r="A2059" t="s">
+        <v>2961</v>
+      </c>
+      <c r="B2059" t="s">
+        <v>2962</v>
+      </c>
+      <c r="C2059" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2059" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2060" spans="1:4">
+      <c r="A2060" t="s">
+        <v>2963</v>
+      </c>
+      <c r="B2060" t="s">
+        <v>1955</v>
+      </c>
+      <c r="C2060" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2060" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2061" spans="1:4">
+      <c r="A2061" t="s">
+        <v>2964</v>
+      </c>
+      <c r="B2061" t="s">
+        <v>2965</v>
+      </c>
+      <c r="C2061" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2061" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2062" spans="1:4">
+      <c r="A2062" t="s">
+        <v>2966</v>
+      </c>
+      <c r="B2062" t="s">
+        <v>2967</v>
+      </c>
+      <c r="C2062" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2062" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2063" spans="1:4">
+      <c r="A2063" t="s">
+        <v>2968</v>
+      </c>
+      <c r="B2063" t="s">
+        <v>2969</v>
+      </c>
+      <c r="C2063" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2063" t="b">
         <v>1</v>
       </c>
     </row>
@@ -37766,6 +38235,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e7156acb-e4b8-4a24-97ff-1280f90be9e8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="10b88064-c9b2-41ef-b928-ffe23b9ecc41" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000ABEC7EA7825F54AB938927CE64AB7F3" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b0cc5dda0475d07cb9b1fc42b0cf1f55">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e7156acb-e4b8-4a24-97ff-1280f90be9e8" xmlns:ns3="10b88064-c9b2-41ef-b928-ffe23b9ecc41" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4483abf1f92f91f7f845c659f7b6f820" ns2:_="" ns3:_="">
     <xsd:import namespace="e7156acb-e4b8-4a24-97ff-1280f90be9e8"/>
@@ -37958,28 +38447,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e7156acb-e4b8-4a24-97ff-1280f90be9e8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="10b88064-c9b2-41ef-b928-ffe23b9ecc41" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7EC2F89-D029-43A5-83BF-73C12B0B37D4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4D12BE6-61F8-42AB-873F-2752C73E7F17}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -37987,5 +38456,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4D12BE6-61F8-42AB-873F-2752C73E7F17}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7EC2F89-D029-43A5-83BF-73C12B0B37D4}"/>
 </file>
</xml_diff>